<commit_message>
Revert "update project members"
This reverts commit 761d532f85a21145ca25f5bab00126fe35aa9ad3.
</commit_message>
<xml_diff>
--- a/Project_Members.xlsx
+++ b/Project_Members.xlsx
@@ -1,124 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26200" windowHeight="13620"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Pratik Mehta</t>
+  </si>
+  <si>
+    <t>Mountain View, CA, USA</t>
+  </si>
+  <si>
     <t>Current City / Country of Residence</t>
   </si>
   <si>
     <t>Time Zone</t>
   </si>
   <si>
+    <t>PST (GMT - 0700 hrs)</t>
+  </si>
+  <si>
     <t>Preferred Contact Email</t>
   </si>
   <si>
+    <t>pratik008@gmail.com</t>
+  </si>
+  <si>
+    <t>Machine Learning, Big Data, Data Science</t>
+  </si>
+  <si>
     <t>Interests</t>
   </si>
   <si>
     <t>Profession</t>
   </si>
   <si>
-    <t>Pratik Mehta</t>
-  </si>
-  <si>
-    <t>Mountain View, CA, USA</t>
-  </si>
-  <si>
-    <t>PST (GMT - 0700 hrs)</t>
-  </si>
-  <si>
-    <t>pratik008@gmail.com</t>
-  </si>
-  <si>
-    <t>Machine Learning, Big Data, Data Science</t>
-  </si>
-  <si>
     <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>Nabin Sharma</t>
-  </si>
-  <si>
-    <t>Providence, RI, USA</t>
-  </si>
-  <si>
-    <t>EST (GMT – 0400 hrs)</t>
-  </si>
-  <si>
-    <t>nabin.s.sharma@gmail.com</t>
-  </si>
-  <si>
-    <t>Data Science, Programming, DSP</t>
-  </si>
-  <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
-    <t>Daniel Maurath</t>
-  </si>
-  <si>
-    <t>San Francisco, CA</t>
-  </si>
-  <si>
-    <t>dmaurath@gmail.com</t>
-  </si>
-  <si>
-    <t>Big Data, Predictive Analytics, Worforce Science</t>
-  </si>
-  <si>
-    <t>Graduate Student in I/O Psychology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,23 +92,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -303,16 +259,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -434,154 +394,71 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="24.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -591,15 +468,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -609,14 +480,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "update project members""
This reverts commit 2374eafef82d7555bd979db47e5497b0db6e8741.
</commit_message>
<xml_diff>
--- a/Project_Members.xlsx
+++ b/Project_Members.xlsx
@@ -1,78 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26200" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Current City / Country of Residence</t>
+  </si>
+  <si>
+    <t>Time Zone</t>
+  </si>
+  <si>
+    <t>Preferred Contact Email</t>
+  </si>
+  <si>
+    <t>Interests</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
     <t>Pratik Mehta</t>
   </si>
   <si>
     <t>Mountain View, CA, USA</t>
   </si>
   <si>
-    <t>Current City / Country of Residence</t>
-  </si>
-  <si>
-    <t>Time Zone</t>
-  </si>
-  <si>
     <t>PST (GMT - 0700 hrs)</t>
   </si>
   <si>
-    <t>Preferred Contact Email</t>
-  </si>
-  <si>
     <t>pratik008@gmail.com</t>
   </si>
   <si>
     <t>Machine Learning, Big Data, Data Science</t>
   </si>
   <si>
-    <t>Interests</t>
-  </si>
-  <si>
-    <t>Profession</t>
-  </si>
-  <si>
     <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Nabin Sharma</t>
+  </si>
+  <si>
+    <t>Providence, RI, USA</t>
+  </si>
+  <si>
+    <t>EST (GMT – 0400 hrs)</t>
+  </si>
+  <si>
+    <t>nabin.s.sharma@gmail.com</t>
+  </si>
+  <si>
+    <t>Data Science, Programming, DSP</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>Daniel Maurath</t>
+  </si>
+  <si>
+    <t>San Francisco, CA</t>
+  </si>
+  <si>
+    <t>dmaurath@gmail.com</t>
+  </si>
+  <si>
+    <t>Big Data, Predictive Analytics, Worforce Science</t>
+  </si>
+  <si>
+    <t>Graduate Student in I/O Psychology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,25 +138,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -259,20 +303,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -394,71 +434,154 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -468,9 +591,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -480,8 +609,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updata project members again
</commit_message>
<xml_diff>
--- a/Project_Members.xlsx
+++ b/Project_Members.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -107,9 +107,6 @@
     <t>jawinquist@gmail.com</t>
   </si>
   <si>
-    <t>ljshope@stanford.kr</t>
-  </si>
-  <si>
     <t>Game Developer</t>
   </si>
   <si>
@@ -150,6 +147,18 @@
   </si>
   <si>
     <t>medical informatics</t>
+  </si>
+  <si>
+    <t>Longbo Qiao</t>
+  </si>
+  <si>
+    <t>Campbell,CA</t>
+  </si>
+  <si>
+    <t>otwick@gmail.com</t>
+  </si>
+  <si>
+    <t>eulerlee@naver.com</t>
   </si>
 </sst>
 </file>
@@ -552,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +665,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -676,12 +685,12 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -690,52 +699,69 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" t="s">
         <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -749,9 +775,10 @@
     <hyperlink ref="D8" r:id="rId7" display="mailto:m.letitbe@gmail.com"/>
     <hyperlink ref="D9" r:id="rId8" display="mailto:lakshmibaskar@gmail.com"/>
     <hyperlink ref="A10" r:id="rId9" display="https://class.coursera.org/datasci-001/forum/profile?user_id=618239"/>
+    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId10"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId11"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Revert "updata project members again"
This reverts commit ef2682e9f696589f48b3eb94e1081d9ca1276476.
</commit_message>
<xml_diff>
--- a/Project_Members.xlsx
+++ b/Project_Members.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -107,6 +107,9 @@
     <t>jawinquist@gmail.com</t>
   </si>
   <si>
+    <t>ljshope@stanford.kr</t>
+  </si>
+  <si>
     <t>Game Developer</t>
   </si>
   <si>
@@ -147,18 +150,6 @@
   </si>
   <si>
     <t>medical informatics</t>
-  </si>
-  <si>
-    <t>Longbo Qiao</t>
-  </si>
-  <si>
-    <t>Campbell,CA</t>
-  </si>
-  <si>
-    <t>otwick@gmail.com</t>
-  </si>
-  <si>
-    <t>eulerlee@naver.com</t>
   </si>
 </sst>
 </file>
@@ -561,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +656,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -685,12 +676,12 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -699,69 +690,52 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -775,10 +749,9 @@
     <hyperlink ref="D8" r:id="rId7" display="mailto:m.letitbe@gmail.com"/>
     <hyperlink ref="D9" r:id="rId8" display="mailto:lakshmibaskar@gmail.com"/>
     <hyperlink ref="A10" r:id="rId9" display="https://class.coursera.org/datasci-001/forum/profile?user_id=618239"/>
-    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId11"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added Sagar Khanna as Project Member
</commit_message>
<xml_diff>
--- a/Project_Members.xlsx
+++ b/Project_Members.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -162,13 +162,28 @@
   </si>
   <si>
     <t>ljshope@stanford.kr</t>
+  </si>
+  <si>
+    <t>Sagar Khanna</t>
+  </si>
+  <si>
+    <t>Noida,UP,India</t>
+  </si>
+  <si>
+    <t>IST (GMT +0530hrs)</t>
+  </si>
+  <si>
+    <t>waves_sagar@yahoo.com</t>
+  </si>
+  <si>
+    <t>Data Science, Analytics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -192,6 +207,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -210,20 +232,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -557,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,6 +783,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -769,9 +814,10 @@
     <hyperlink ref="D8" r:id="rId7" display="mailto:m.letitbe@gmail.com"/>
     <hyperlink ref="D9" r:id="rId8" display="mailto:lakshmibaskar@gmail.com"/>
     <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId10"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId11"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>